<commit_message>
Test Plan is uploaded
</commit_message>
<xml_diff>
--- a/Doc/GPIO_VIP_test_plan.xlsx
+++ b/Doc/GPIO_VIP_test_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan\gpio_vip\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,32 +29,81 @@
     <t>Sl.No</t>
   </si>
   <si>
-    <t>Test Cases to be built on the property</t>
-  </si>
-  <si>
     <t>Test Plan for GPIO VIP</t>
   </si>
   <si>
-    <t>To set the number of pins per port.</t>
-  </si>
-  <si>
-    <t>To set the direction register as it can be configured as both input and output.</t>
-  </si>
-  <si>
-    <t>To Check the interrupt Configuration Register</t>
-  </si>
-  <si>
-    <t>To set the Interrupt Configuration Register</t>
-  </si>
-  <si>
-    <t>To select the function of the port pin and set it for the general purpose or interrupt handling</t>
+    <r>
+      <t xml:space="preserve">To set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Direction Register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as it can be configured as both input and output.</t>
+    </r>
+  </si>
+  <si>
+    <t>To set the number of pins per port and also configure number of available ports.</t>
+  </si>
+  <si>
+    <t>To select the function of the port pin and set it for the general purpose or interrupt handling.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interrupt Configuration Register.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To Check the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interrupt Configuration Register.</t>
+    </r>
+  </si>
+  <si>
+    <t>Properties to be Evaluated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +117,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -110,13 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,7 +475,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,57 +484,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3"/>
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the test plan
</commit_message>
<xml_diff>
--- a/Doc/GPIO_VIP_test_plan.xlsx
+++ b/Doc/GPIO_VIP_test_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sl.No</t>
   </si>
@@ -97,6 +97,84 @@
   </si>
   <si>
     <t>Properties to be Evaluated</t>
+  </si>
+  <si>
+    <r>
+      <t>To set and check the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Write data pin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when port direction is set as input.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>To set and check the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Read data pin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when port direction is set as output.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To enable or disable the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pull up or pull down</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> configuration</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -182,14 +260,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -472,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,57 +562,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>